<commit_message>
Added Coulson et al 2008 dataset
</commit_message>
<xml_diff>
--- a/datasheets/Stoskopf_et_al_2001.xlsx
+++ b/datasheets/Stoskopf_et_al_2001.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t xml:space="preserve">Collection number</t>
   </si>
@@ -130,9 +130,6 @@
     <t xml:space="preserve">refShort</t>
   </si>
   <si>
-    <t xml:space="preserve">Captive individual 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Alligator mississipiensis</t>
   </si>
   <si>
@@ -170,9 +167,6 @@
   </si>
   <si>
     <t xml:space="preserve">Stoskopf et al. (2001)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wild individual 1</t>
   </si>
   <si>
     <t xml:space="preserve">bone, thoracic vertebra</t>
@@ -354,8 +348,8 @@
   </sheetPr>
   <dimension ref="A1:AJ27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Z1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH14" activeCellId="0" sqref="AH14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,35 +495,33 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="K2" s="6" t="n">
         <v>19.1925</v>
@@ -538,7 +530,7 @@
         <v>0.6675</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>-3.6</v>
@@ -601,45 +593,43 @@
         <v>-3.2</v>
       </c>
       <c r="AH2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="K3" s="6" t="n">
         <v>21.09125</v>
@@ -648,7 +638,7 @@
         <v>1.335</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N3" s="5" t="n">
         <v>-3.7</v>
@@ -713,13 +703,13 @@
         <v>-4.6</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>